<commit_message>
Add and update examples
</commit_message>
<xml_diff>
--- a/Examples/Data/Formatting/ComputeColorChoosenByMSExcel/Book1.xlsx
+++ b/Examples/Data/Formatting/ComputeColorChoosenByMSExcel/Book1.xlsx
@@ -53,16 +53,21 @@
   <dxfs count="2">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <color auto="1"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>

</xml_diff>